<commit_message>
Updated to display and detect YouTube video
</commit_message>
<xml_diff>
--- a/extras/sample-form/YouTube detector sample form.xlsx
+++ b/extras/sample-form/YouTube detector sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/youtube-detector/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961506F4-B72F-6B41-B5EB-AFC275805D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC2FEC-219B-B847-B5BE-DCFD7B41350E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31700" yWindow="-1680" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1520" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="378">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2604,20 +2604,33 @@
     <t/>
   </si>
   <si>
-    <t>example1</t>
-  </si>
-  <si>
     <t>YouTube detector sample form</t>
   </si>
   <si>
     <t>youtube_detector_sample_form</t>
   </si>
   <si>
+    <t>custom-youtube-detector(video='VmGM-jlAqIw')</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Check out this video:&lt;/p&gt;
-&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/VmGM-jlAqIw" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>custom-youtube-detector</t>
+&lt;div id="player"&gt;&lt;/div&gt;
+&lt;p&gt;Did you watch the video?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>embedded_video</t>
+  </si>
+  <si>
+    <t>disp_watch_time</t>
+  </si>
+  <si>
+    <t>watch_time</t>
+  </si>
+  <si>
+    <t>int(plug-in-metadata(${embedded_video}) div 1000)</t>
+  </si>
+  <si>
+    <t>The video was watched for ${watch_time} seconds.</t>
   </si>
 </sst>
 </file>
@@ -4767,13 +4780,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4969,21 +4982,43 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="170" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>306</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>372</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>377</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -5277,14 +5312,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>371</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2107232047</v>
+        <v>2107232116</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>368</v>

</xml_diff>

<commit_message>
Added check if video ended
</commit_message>
<xml_diff>
--- a/extras/sample-form/YouTube detector sample form.xlsx
+++ b/extras/sample-form/YouTube detector sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/youtube-detector/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC2FEC-219B-B847-B5BE-DCFD7B41350E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598540E8-3493-BC48-89DD-9981A441FE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1520" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32080" yWindow="-3020" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="392">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2613,24 +2613,74 @@
     <t>custom-youtube-detector(video='VmGM-jlAqIw')</t>
   </si>
   <si>
-    <t>&lt;p&gt;Check out this video:&lt;/p&gt;
+    <t>disp_watch_time</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this field, if you leave, come back, and play the video again, the time watched will restart.&lt;/p&gt;
+&lt;p&gt;Check out this video:&lt;/p&gt;
 &lt;div id="player"&gt;&lt;/div&gt;
 &lt;p&gt;Did you watch the video?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>embedded_video</t>
-  </si>
-  <si>
-    <t>disp_watch_time</t>
-  </si>
-  <si>
-    <t>watch_time</t>
-  </si>
-  <si>
-    <t>int(plug-in-metadata(${embedded_video}) div 1000)</t>
-  </si>
-  <si>
-    <t>The video was watched for ${watch_time} seconds.</t>
+    <t>&lt;p&gt;In this field, if you leave and come back, the time spent already watching the video will be saved.&lt;/p&gt;
+&lt;p&gt;Check out this video:&lt;/p&gt;
+&lt;div id="player"&gt;&lt;/div&gt;
+&lt;p&gt;Did you watch the video?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>saved_time</t>
+  </si>
+  <si>
+    <t>not_saved_if_restart</t>
+  </si>
+  <si>
+    <t>watch_time1</t>
+  </si>
+  <si>
+    <t>watch_time2</t>
+  </si>
+  <si>
+    <t>disp_watch_time2</t>
+  </si>
+  <si>
+    <t>custom-youtube-detector(video='VmGM-jlAqIw', reset=1)</t>
+  </si>
+  <si>
+    <t>metadata1</t>
+  </si>
+  <si>
+    <t>metadata2</t>
+  </si>
+  <si>
+    <t>ended2</t>
+  </si>
+  <si>
+    <t>ended1</t>
+  </si>
+  <si>
+    <t>int(selected-at(${metadata1}, 0) div 1000)</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${saved_time})</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${not_saved_if_restart})</t>
+  </si>
+  <si>
+    <t>if(selected-at(${metadata2}, 1) = '1', 'Yes', 'No')</t>
+  </si>
+  <si>
+    <t>if(selected-at(${metadata1}, 1) = '1', 'Yes', 'No')</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Second video&lt;/p&gt;
+&lt;p&gt;Watch time: ${watch_time2}&lt;br&gt;
+Ended: ${ended2}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;First video&lt;/p&gt;
+&lt;p&gt;Watch time: ${watch_time1}&lt;br&gt;
+Ended: ${ended1}&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4780,13 +4830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4982,15 +5032,15 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>306</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>371</v>
@@ -5003,21 +5053,101 @@
         <v>149</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="N13" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="C18" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>377</v>
+      <c r="B22" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -5319,7 +5449,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2107232116</v>
+        <v>2107272030</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>368</v>

</xml_diff>

<commit_message>
Fixed retrieval of time watched
</commit_message>
<xml_diff>
--- a/extras/sample-form/YouTube detector sample form.xlsx
+++ b/extras/sample-form/YouTube detector sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/youtube-detector/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598540E8-3493-BC48-89DD-9981A441FE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F985C6E-601C-534E-A399-9674BF8AF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32080" yWindow="-3020" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32080" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="393">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2658,9 +2658,6 @@
     <t>ended1</t>
   </si>
   <si>
-    <t>int(selected-at(${metadata1}, 0) div 1000)</t>
-  </si>
-  <si>
     <t>plug-in-metadata(${saved_time})</t>
   </si>
   <si>
@@ -2681,6 +2678,12 @@
     <t>&lt;p&gt;First video&lt;/p&gt;
 &lt;p&gt;Watch time: ${watch_time1}&lt;br&gt;
 Ended: ${ended1}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>round(selected-at(${metadata1}, 0) div 1000, 0)</t>
+  </si>
+  <si>
+    <t>round(selected-at(${metadata2}, 0) div 1000, 0)</t>
   </si>
 </sst>
 </file>
@@ -4833,7 +4836,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
@@ -5056,7 +5059,7 @@
         <v>381</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5067,7 +5070,7 @@
         <v>377</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -5078,7 +5081,7 @@
         <v>384</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="68" x14ac:dyDescent="0.2">
@@ -5089,7 +5092,7 @@
         <v>372</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -5114,7 +5117,7 @@
         <v>382</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -5125,7 +5128,7 @@
         <v>378</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -5136,7 +5139,7 @@
         <v>383</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5147,7 +5150,7 @@
         <v>379</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5449,7 +5452,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2107272030</v>
+        <v>2108021152</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>368</v>

</xml_diff>

<commit_message>
Updated sample form to reflect timing
</commit_message>
<xml_diff>
--- a/extras/sample-form/YouTube detector sample form.xlsx
+++ b/extras/sample-form/YouTube detector sample form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/youtube-detector/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109B9477-3C25-6249-95AF-810F3E6BE5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F158F19-F665-0E45-884F-869F9FC63C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29880" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="500" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2668,12 +2668,6 @@
 Ended: ${ended1}&lt;/p&gt;</t>
   </si>
   <si>
-    <t>round(selected-at(${metadata1}, 0) div 1000, 0)</t>
-  </si>
-  <si>
-    <t>round(selected-at(${metadata2}, 0) div 1000, 0)</t>
-  </si>
-  <si>
     <t>autoplay_video</t>
   </si>
   <si>
@@ -2695,9 +2689,6 @@
     <t>&lt;p&gt;Third video&lt;/p&gt;
 &lt;p&gt;Watch time: ${watch_time3}&lt;br&gt;
 Ended: ${ended3}&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>round(selected-at(${metadata3}, 0) div 1000, 0)</t>
   </si>
   <si>
     <t>if(selected-at(${metadata3}, 1) = '1', 'Yes', 'No')</t>
@@ -2725,6 +2716,15 @@
 &lt;p&gt;Check out this video:&lt;/p&gt;
 &lt;div id="player"&gt;&lt;/div&gt;
 &lt;p&gt;Did you watch the video?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>round(selected-at(${metadata2}, 0), 0)</t>
+  </si>
+  <si>
+    <t>round(selected-at(${metadata3}, 0), 0)</t>
+  </si>
+  <si>
+    <t>round(selected-at(${metadata1}, 0), 0)</t>
   </si>
 </sst>
 </file>
@@ -3433,277 +3433,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="169">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="134">
     <dxf>
       <fill>
         <patternFill>
@@ -5147,7 +4877,7 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
@@ -5354,7 +5084,7 @@
         <v>373</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>371</v>
@@ -5381,7 +5111,7 @@
         <v>375</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -5411,13 +5141,13 @@
         <v>306</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -5428,7 +5158,7 @@
         <v>380</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -5439,7 +5169,7 @@
         <v>376</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -5472,7 +5202,7 @@
         <v>374</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>378</v>
@@ -5483,7 +5213,7 @@
         <v>149</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="N25" s="9" t="s">
         <v>384</v>
@@ -5494,10 +5224,10 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -5505,10 +5235,10 @@
         <v>148</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5516,147 +5246,147 @@
         <v>42</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="168" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 O1:O1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="167" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="166" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="165" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="164" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="163" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="162" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="161" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="20" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="158" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="157" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="156" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="155" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="154" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="5" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="9" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="11" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="15" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="19" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="21" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="23" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="25" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="28" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="42" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="44" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="45" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="47" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="48" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="50" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="135" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="134" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5763,7 +5493,7 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="133" priority="1">
+    <cfRule type="expression" dxfId="98" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5821,7 +5551,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2108021320</v>
+        <v>2108100112</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>368</v>
@@ -6413,7 +6143,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>
@@ -9657,348 +9387,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="132" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="131" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="130" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="129" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="128" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="127" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="126" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="125" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="122" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="121" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="120" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="119" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="118" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="100" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="99" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="81" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="80" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="79" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="75" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="74" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="73" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="72" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>